<commit_message>
Informe de resultados updated
</commit_message>
<xml_diff>
--- a/Documentacion/Informe de resultados.xlsx
+++ b/Documentacion/Informe de resultados.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="38">
   <si>
     <t>Fenómeno, sistema o proceso:</t>
   </si>
@@ -77,7 +77,7 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve">2 * 3 * 3 * 3 = </t>
+      <t xml:space="preserve">2 * 3 * 4 * 3 = </t>
     </r>
     <r>
       <rPr>
@@ -85,7 +85,7 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>54</t>
+      <t>72</t>
     </r>
   </si>
   <si>
@@ -125,16 +125,19 @@
     <t xml:space="preserve">Ascendente </t>
   </si>
   <si>
-    <t>10^5</t>
+    <t>10^3</t>
   </si>
   <si>
     <t>Descendente</t>
   </si>
   <si>
-    <t>10^10</t>
+    <t>10^4</t>
   </si>
   <si>
     <t>Aleatorio</t>
+  </si>
+  <si>
+    <t>10^6</t>
   </si>
   <si>
     <t>tamaño del arreglo</t>
@@ -164,14 +167,14 @@
       <name val="Roboto"/>
     </font>
     <font>
-      <name val="Arial"/>
-    </font>
-    <font/>
-    <font>
       <b/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <name val="Arial"/>
+    </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -227,27 +230,27 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -534,15 +537,15 @@
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -550,7 +553,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -558,7 +561,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -569,7 +572,7 @@
       <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="6">
         <f>3</f>
         <v>3</v>
       </c>
@@ -605,59 +608,59 @@
   </cols>
   <sheetData>
     <row r="5">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="10" t="s">
+      <c r="B6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="10" t="s">
+      <c r="B7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="3"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="10" t="s">
+      <c r="B11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -665,8 +668,8 @@
       <c r="B12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="10" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -674,9 +677,14 @@
       <c r="B13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="10" t="s">
-        <v>35</v>
+      <c r="C13" s="3"/>
+      <c r="D13" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -701,128 +709,128 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="13" t="s">
+      <c r="B3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="B4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="B5" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>33</v>
       </c>
     </row>
@@ -845,10 +853,10 @@
         <v>23</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>31</v>
@@ -859,10 +867,10 @@
         <v>23</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>33</v>
@@ -873,10 +881,10 @@
         <v>23</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>35</v>
@@ -890,121 +898,121 @@
         <v>26</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="13" t="s">
+      <c r="B18" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>27</v>
+      <c r="B21" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>27</v>
+      <c r="B22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>27</v>
+      <c r="B23" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E23" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1013,10 +1021,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>31</v>
@@ -1027,10 +1035,10 @@
         <v>23</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>33</v>
@@ -1041,150 +1049,150 @@
         <v>23</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="13" t="s">
+      <c r="B27" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="13" t="s">
+      <c r="B28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30">
-      <c r="B30" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>24</v>
+      <c r="B30" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>24</v>
+      <c r="B31" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>24</v>
+      <c r="B32" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E32" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>24</v>
+      <c r="B33" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>24</v>
+      <c r="B34" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35">
-      <c r="B35" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>24</v>
+      <c r="B35" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>31</v>
@@ -1192,13 +1200,13 @@
     </row>
     <row r="37">
       <c r="B37" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>33</v>
@@ -1206,24 +1214,24 @@
     </row>
     <row r="38">
       <c r="B38" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="39">
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>30</v>
@@ -1233,11 +1241,11 @@
       </c>
     </row>
     <row r="40">
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>30</v>
@@ -1247,11 +1255,11 @@
       </c>
     </row>
     <row r="41">
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D41" s="13" t="s">
         <v>30</v>
@@ -1261,11 +1269,11 @@
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>32</v>
@@ -1275,11 +1283,11 @@
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D43" s="13" t="s">
         <v>32</v>
@@ -1289,11 +1297,11 @@
       </c>
     </row>
     <row r="44">
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D44" s="13" t="s">
         <v>32</v>
@@ -1303,11 +1311,11 @@
       </c>
     </row>
     <row r="45">
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D45" s="13" t="s">
         <v>34</v>
@@ -1317,11 +1325,11 @@
       </c>
     </row>
     <row r="46">
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D46" s="13" t="s">
         <v>34</v>
@@ -1331,11 +1339,11 @@
       </c>
     </row>
     <row r="47">
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D47" s="13" t="s">
         <v>34</v>
@@ -1345,128 +1353,380 @@
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="49">
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="50">
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51">
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="52">
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E52" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="53">
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="54">
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E54" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="55">
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D55" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E55" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="56">
-      <c r="B56" s="13" t="s">
+      <c r="B56" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E56" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E62" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E64" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E65" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D67" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E74" s="12" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test results added to doc
</commit_message>
<xml_diff>
--- a/Documentacion/Informe de resultados.xlsx
+++ b/Documentacion/Informe de resultados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10\Desktop\SortExperimentsDesign\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\ExperimentsDesign\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324072B4-4432-4CD7-8D5B-0A04F74E9BEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E2FCE8-67AC-4042-B6DC-56A53E31C7C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Informe" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,22 @@
     <sheet name="Tiempos" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="73">
   <si>
     <t>Fenómeno, sistema o proceso:</t>
   </si>
@@ -222,6 +233,54 @@
   </si>
   <si>
     <t>1min</t>
+  </si>
+  <si>
+    <t>44ms</t>
+  </si>
+  <si>
+    <t>1ms</t>
+  </si>
+  <si>
+    <t>6ms</t>
+  </si>
+  <si>
+    <t>396ms</t>
+  </si>
+  <si>
+    <t>443ms</t>
+  </si>
+  <si>
+    <t>37,7min</t>
+  </si>
+  <si>
+    <t>39,7min</t>
+  </si>
+  <si>
+    <t>49ms</t>
+  </si>
+  <si>
+    <t>11ms</t>
+  </si>
+  <si>
+    <t>54ms</t>
+  </si>
+  <si>
+    <t>46ms</t>
+  </si>
+  <si>
+    <t>113ms</t>
+  </si>
+  <si>
+    <t>13ms</t>
+  </si>
+  <si>
+    <t>59ms</t>
+  </si>
+  <si>
+    <t>654ms</t>
+  </si>
+  <si>
+    <t>1,2min</t>
   </si>
 </sst>
 </file>
@@ -505,10 +564,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -535,6 +590,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,87 +816,87 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="31.6640625" customWidth="1"/>
+    <col min="8" max="8" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:8" ht="12.75">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-    </row>
-    <row r="4" spans="2:8">
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" spans="2:8" ht="12.75">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="2:8">
+      <c r="D4" s="25"/>
+    </row>
+    <row r="5" spans="2:8" ht="12.75">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="2:8">
+      <c r="D5" s="25"/>
+    </row>
+    <row r="6" spans="2:8" ht="12.75">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
     </row>
     <row r="7" spans="2:8" ht="15.75" customHeight="1">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="C8" s="15" t="s">
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="2:8" ht="12.75">
+      <c r="C8" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="C9" s="15" t="s">
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="2:8" ht="12.75">
+      <c r="C9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:8">
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="2:8" ht="12.75">
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
@@ -849,27 +908,27 @@
       <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="2:8">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+    </row>
+    <row r="12" spans="2:8" ht="12.75">
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="2:8">
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+    </row>
+    <row r="13" spans="2:8" ht="12.75">
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
@@ -877,7 +936,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" ht="12.75">
       <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
@@ -911,10 +970,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="2:4">
@@ -1011,12 +1070,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
@@ -2050,1166 +2109,1214 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E79D4DC-B0A6-4027-86C8-DEE4E9C7BA61}">
   <dimension ref="B3:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53:F64"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="36.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="32.44140625" customWidth="1"/>
-    <col min="6" max="6" width="30.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="13.8" thickBot="1">
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B4" s="16" t="s">
+    <row r="3" spans="2:6" ht="13.5" thickBot="1">
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B5" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="20" t="s">
+    <row r="5" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B6" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="25"/>
-    </row>
-    <row r="7" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B7" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B8" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="20" t="s">
+      <c r="F5" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B6" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="25"/>
-    </row>
-    <row r="9" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="23"/>
-    </row>
-    <row r="10" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B10" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="23"/>
-    </row>
-    <row r="11" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B11" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="F8" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="25"/>
-    </row>
-    <row r="12" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B12" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="23"/>
-    </row>
-    <row r="13" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B13" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="25"/>
-    </row>
-    <row r="14" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B14" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="20" t="s">
+      <c r="F11" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B14" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="23"/>
-    </row>
-    <row r="15" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B15" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="23"/>
-    </row>
-    <row r="16" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B16" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F16" s="25"/>
-    </row>
-    <row r="17" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B17" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="20" t="s">
+      <c r="F14" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B17" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B18" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" s="23" t="s">
+    <row r="18" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B18" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B19" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="23" t="s">
+    <row r="19" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B19" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B20" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="20" t="s">
+    <row r="20" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B20" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B21" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="23" t="s">
+    <row r="21" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B21" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B22" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="25" t="s">
+    <row r="22" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B22" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B23" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="20" t="s">
+    <row r="23" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B23" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B24" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="23" t="s">
+    <row r="24" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B24" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B25" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="25" t="s">
+    <row r="25" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B25" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B26" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="20" t="s">
+    <row r="26" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B26" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B27" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="23" t="s">
+    <row r="27" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B27" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B28" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F28" s="23" t="s">
+    <row r="28" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="19" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B29" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="20" t="s">
+    <row r="29" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B29" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="23"/>
-    </row>
-    <row r="30" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B30" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="25"/>
-    </row>
-    <row r="31" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B31" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F31" s="25"/>
-    </row>
-    <row r="32" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B32" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="20" t="s">
+      <c r="F29" s="19"/>
+    </row>
+    <row r="30" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B30" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="21"/>
+    </row>
+    <row r="31" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B31" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="21"/>
+    </row>
+    <row r="32" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B32" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="23"/>
-    </row>
-    <row r="33" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B33" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="25"/>
-    </row>
-    <row r="34" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B34" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" s="25"/>
-    </row>
-    <row r="35" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B35" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="20" t="s">
+      <c r="F32" s="19"/>
+    </row>
+    <row r="33" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B33" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="21"/>
+    </row>
+    <row r="34" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B34" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="21"/>
+    </row>
+    <row r="35" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B35" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F35" s="23"/>
-    </row>
-    <row r="36" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B36" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F36" s="25"/>
-    </row>
-    <row r="37" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B37" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F37" s="23"/>
-    </row>
-    <row r="38" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B38" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" s="20" t="s">
+      <c r="F35" s="19"/>
+    </row>
+    <row r="36" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B36" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E36" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" s="21"/>
+    </row>
+    <row r="37" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B37" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="19"/>
+    </row>
+    <row r="38" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B38" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="24"/>
-    </row>
-    <row r="39" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B39" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F39" s="22"/>
-    </row>
-    <row r="40" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B40" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F40" s="25"/>
-    </row>
-    <row r="41" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B41" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E41" s="20" t="s">
+      <c r="F38" s="20"/>
+    </row>
+    <row r="39" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B39" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B40" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" s="21"/>
+    </row>
+    <row r="41" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B41" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E41" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F41" s="23"/>
-    </row>
-    <row r="42" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B42" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F42" s="23"/>
-    </row>
-    <row r="43" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B43" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F43" s="25"/>
-    </row>
-    <row r="44" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B44" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E44" s="20" t="s">
+      <c r="F41" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B42" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B43" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B44" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F44" s="25"/>
-    </row>
-    <row r="45" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B45" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="23"/>
-    </row>
-    <row r="46" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B46" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F46" s="25"/>
-    </row>
-    <row r="47" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B47" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E47" s="20" t="s">
+      <c r="F44" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B45" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B46" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B47" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F47" s="23"/>
-    </row>
-    <row r="48" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B48" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F48" s="23"/>
-    </row>
-    <row r="49" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B49" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F49" s="25"/>
-    </row>
-    <row r="50" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B50" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C50" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E50" s="27" t="s">
+      <c r="F47" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B48" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E48" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B49" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B50" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E50" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="F50" s="23"/>
-    </row>
-    <row r="51" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B51" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E51" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F51" s="23"/>
-    </row>
-    <row r="52" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B52" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E52" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F52" s="25"/>
-    </row>
-    <row r="53" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B53" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C53" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E53" s="20" t="s">
+      <c r="F50" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B51" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B52" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F52" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B53" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F53" s="25" t="s">
+      <c r="F53" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B54" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E54" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F54" s="24" t="s">
+    <row r="54" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B54" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F54" s="20" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B55" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F55" s="25" t="s">
+    <row r="55" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B55" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F55" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B56" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="20" t="s">
+    <row r="56" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B56" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E56" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F56" s="25" t="s">
+      <c r="F56" s="21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B57" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D57" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F57" s="25" t="s">
+    <row r="57" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B57" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F57" s="21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B58" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F58" s="23" t="s">
+    <row r="58" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B58" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B59" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D59" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" s="20" t="s">
+    <row r="59" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B59" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F59" s="23" t="s">
+      <c r="F59" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B60" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D60" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F60" s="23" t="s">
+    <row r="60" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B60" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B61" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D61" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F61" s="25" t="s">
+    <row r="61" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B61" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F61" s="21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B62" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D62" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E62" s="20" t="s">
+    <row r="62" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B62" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E62" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F62" s="23" t="s">
+      <c r="F62" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B63" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C63" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E63" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F63" s="23" t="s">
+    <row r="63" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B63" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F63" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B64" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C64" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E64" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F64" s="23" t="s">
+    <row r="64" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B64" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F64" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B65" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C65" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D65" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E65" s="20" t="s">
+    <row r="65" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B65" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E65" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F65" s="24"/>
-    </row>
-    <row r="66" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B66" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D66" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E66" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F66" s="22"/>
-    </row>
-    <row r="67" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B67" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D67" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E67" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F67" s="22"/>
-    </row>
-    <row r="68" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B68" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E68" s="20" t="s">
+      <c r="F65" s="20"/>
+    </row>
+    <row r="66" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B66" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E66" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F66" s="18"/>
+    </row>
+    <row r="67" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B67" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E67" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F67" s="18"/>
+    </row>
+    <row r="68" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B68" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F68" s="22"/>
-    </row>
-    <row r="69" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B69" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C69" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E69" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F69" s="25"/>
-    </row>
-    <row r="70" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B70" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C70" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D70" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E70" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F70" s="23"/>
-    </row>
-    <row r="71" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B71" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C71" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D71" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E71" s="20" t="s">
+      <c r="F68" s="18"/>
+    </row>
+    <row r="69" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B69" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F69" s="21"/>
+    </row>
+    <row r="70" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B70" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F70" s="19"/>
+    </row>
+    <row r="71" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B71" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F71" s="23"/>
-    </row>
-    <row r="72" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B72" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C72" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D72" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E72" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F72" s="23"/>
-    </row>
-    <row r="73" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B73" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C73" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D73" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E73" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F73" s="25"/>
-    </row>
-    <row r="74" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B74" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C74" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D74" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E74" s="20" t="s">
+      <c r="F71" s="19"/>
+    </row>
+    <row r="72" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B72" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F72" s="19"/>
+    </row>
+    <row r="73" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B73" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F73" s="21"/>
+    </row>
+    <row r="74" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B74" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E74" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F74" s="23"/>
-    </row>
-    <row r="75" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B75" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C75" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D75" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E75" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="F75" s="23"/>
-    </row>
-    <row r="76" spans="2:6" ht="13.8" thickBot="1">
-      <c r="B76" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C76" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="F76" s="23"/>
+      <c r="F74" s="19"/>
+    </row>
+    <row r="75" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B75" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E75" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F75" s="19"/>
+    </row>
+    <row r="76" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B76" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E76" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F76" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Documentation and time update
</commit_message>
<xml_diff>
--- a/Documentacion/Informe de resultados.xlsx
+++ b/Documentacion/Informe de resultados.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\ExperimentsDesign\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prestamo\Documents\Integrador\SortExperimentsDesign\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E2FCE8-67AC-4042-B6DC-56A53E31C7C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Informe" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Tratamientos" sheetId="3" r:id="rId3"/>
     <sheet name="Tiempos" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="88">
   <si>
     <t>Fenómeno, sistema o proceso:</t>
   </si>
@@ -98,6 +97,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">2 * 3 * 4 * 3 = </t>
     </r>
@@ -107,6 +107,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>72</t>
     </r>
@@ -282,11 +283,56 @@
   <si>
     <t>1,2min</t>
   </si>
+  <si>
+    <t>9 ms</t>
+  </si>
+  <si>
+    <t>&lt; 1ms</t>
+  </si>
+  <si>
+    <t>583 ms</t>
+  </si>
+  <si>
+    <t>115 ms</t>
+  </si>
+  <si>
+    <t>10 ms</t>
+  </si>
+  <si>
+    <t>46 ms</t>
+  </si>
+  <si>
+    <t>8 ms</t>
+  </si>
+  <si>
+    <t>42 ms</t>
+  </si>
+  <si>
+    <t>80 ms</t>
+  </si>
+  <si>
+    <t>28,3 min</t>
+  </si>
+  <si>
+    <t>163 m</t>
+  </si>
+  <si>
+    <t>1 ms</t>
+  </si>
+  <si>
+    <t>25,5 min</t>
+  </si>
+  <si>
+    <t>165 ms</t>
+  </si>
+  <si>
+    <t>1 min</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -297,11 +343,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -313,14 +361,17 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -808,7 +859,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -962,7 +1013,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1062,13 +1113,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="B2:E74"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="C1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -2106,11 +2157,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E79D4DC-B0A6-4027-86C8-DEE4E9C7BA61}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="D65" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -2563,7 +2614,9 @@
       <c r="E29" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="19"/>
+      <c r="F29" s="19" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="30" spans="2:6" ht="13.5" thickBot="1">
       <c r="B30" s="14" t="s">
@@ -2578,7 +2631,9 @@
       <c r="E30" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="21"/>
+      <c r="F30" s="21" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="31" spans="2:6" ht="13.5" thickBot="1">
       <c r="B31" s="14" t="s">
@@ -2593,7 +2648,9 @@
       <c r="E31" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="21" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="32" spans="2:6" ht="13.5" thickBot="1">
       <c r="B32" s="14" t="s">
@@ -2608,7 +2665,9 @@
       <c r="E32" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="19"/>
+      <c r="F32" s="19" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="33" spans="2:6" ht="13.5" thickBot="1">
       <c r="B33" s="14" t="s">
@@ -2623,7 +2682,9 @@
       <c r="E33" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="21" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="34" spans="2:6" ht="13.5" thickBot="1">
       <c r="B34" s="14" t="s">
@@ -2638,7 +2699,9 @@
       <c r="E34" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="21" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="35" spans="2:6" ht="13.5" thickBot="1">
       <c r="B35" s="14" t="s">
@@ -2653,7 +2716,9 @@
       <c r="E35" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F35" s="19"/>
+      <c r="F35" s="19" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="36" spans="2:6" ht="13.5" thickBot="1">
       <c r="B36" s="14" t="s">
@@ -2668,7 +2733,9 @@
       <c r="E36" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="21"/>
+      <c r="F36" s="21" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="37" spans="2:6" ht="13.5" thickBot="1">
       <c r="B37" s="14" t="s">
@@ -2683,7 +2750,9 @@
       <c r="E37" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="19"/>
+      <c r="F37" s="19" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="38" spans="2:6" ht="13.5" thickBot="1">
       <c r="B38" s="14" t="s">
@@ -2698,7 +2767,9 @@
       <c r="E38" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="20"/>
+      <c r="F38" s="20" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="39" spans="2:6" ht="13.5" thickBot="1">
       <c r="B39" s="14" t="s">
@@ -2713,7 +2784,9 @@
       <c r="E39" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="18"/>
+      <c r="F39" s="18" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="40" spans="2:6" ht="13.5" thickBot="1">
       <c r="B40" s="14" t="s">
@@ -2728,7 +2801,9 @@
       <c r="E40" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="21"/>
+      <c r="F40" s="21" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="41" spans="2:6" ht="13.5" thickBot="1">
       <c r="B41" s="14" t="s">
@@ -3151,7 +3226,9 @@
       <c r="E65" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F65" s="20"/>
+      <c r="F65" s="20" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="66" spans="2:6" ht="13.5" thickBot="1">
       <c r="B66" s="14" t="s">
@@ -3166,7 +3243,9 @@
       <c r="E66" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F66" s="18"/>
+      <c r="F66" s="18" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="67" spans="2:6" ht="13.5" thickBot="1">
       <c r="B67" s="14" t="s">
@@ -3181,7 +3260,9 @@
       <c r="E67" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F67" s="18"/>
+      <c r="F67" s="18" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="68" spans="2:6" ht="13.5" thickBot="1">
       <c r="B68" s="14" t="s">
@@ -3196,7 +3277,9 @@
       <c r="E68" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F68" s="18"/>
+      <c r="F68" s="18" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="69" spans="2:6" ht="13.5" thickBot="1">
       <c r="B69" s="14" t="s">
@@ -3211,7 +3294,9 @@
       <c r="E69" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F69" s="21"/>
+      <c r="F69" s="21" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="70" spans="2:6" ht="13.5" thickBot="1">
       <c r="B70" s="14" t="s">
@@ -3226,7 +3311,9 @@
       <c r="E70" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F70" s="19"/>
+      <c r="F70" s="19" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="71" spans="2:6" ht="13.5" thickBot="1">
       <c r="B71" s="14" t="s">
@@ -3241,7 +3328,9 @@
       <c r="E71" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F71" s="19"/>
+      <c r="F71" s="19" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="72" spans="2:6" ht="13.5" thickBot="1">
       <c r="B72" s="14" t="s">
@@ -3256,7 +3345,9 @@
       <c r="E72" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F72" s="19"/>
+      <c r="F72" s="19" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="73" spans="2:6" ht="13.5" thickBot="1">
       <c r="B73" s="14" t="s">
@@ -3271,7 +3362,9 @@
       <c r="E73" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F73" s="21"/>
+      <c r="F73" s="21" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="74" spans="2:6" ht="13.5" thickBot="1">
       <c r="B74" s="14" t="s">
@@ -3286,7 +3379,9 @@
       <c r="E74" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F74" s="19"/>
+      <c r="F74" s="19" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="75" spans="2:6" ht="13.5" thickBot="1">
       <c r="B75" s="14" t="s">
@@ -3301,7 +3396,9 @@
       <c r="E75" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F75" s="19"/>
+      <c r="F75" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="76" spans="2:6" ht="13.5" thickBot="1">
       <c r="B76" s="14" t="s">
@@ -3316,7 +3413,9 @@
       <c r="E76" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F76" s="19"/>
+      <c r="F76" s="19" t="s">
+        <v>75</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>